<commit_message>
change RGB LED to 5V, add level shifter, change thickness of PCB to 1.0mm, add simple box with FreeCad, update readme
</commit_message>
<xml_diff>
--- a/bom/ps4-usb-hen-esp32-jlcpcb.xlsx
+++ b/bom/ps4-usb-hen-esp32-jlcpcb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Tofi\github\PS4-USB-HEN-ESP32\ps4-usb-hen-esp32\gerber\X\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Tofi\github\PS4-USB-HEN-ESP32\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ps4-usb-hen-esp32" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Comment</t>
   </si>
@@ -128,12 +128,6 @@
     <t>C10418</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R1, R2, R5, R6, R7, R8, R9, R10, R11</t>
-  </si>
-  <si>
     <t>R_0603_1608Metric</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>SW1, SW2</t>
   </si>
   <si>
-    <t>Button_Switch_SMD:SW_SPST_TL3342</t>
-  </si>
-  <si>
     <t xml:space="preserve">C318884 </t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Package_TO_SOT_SMD:SOT-23-6</t>
-  </si>
-  <si>
     <t xml:space="preserve">C85364 </t>
   </si>
   <si>
@@ -200,13 +188,34 @@
     <t>U3</t>
   </si>
   <si>
-    <t>RF_Module:ESP32-S2-WROVER</t>
-  </si>
-  <si>
     <t xml:space="preserve">C701333 </t>
   </si>
   <si>
     <t>C1, C2, C3, C4, C6, C8,C9</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R5, R6, R7, R8, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>C8545</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>SW_SPST_TL3342</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
 </sst>
 </file>
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -574,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -683,99 +692,113 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>